<commit_message>
Sprint 3 Acceptance Criteria Added
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhruv/IdeaProjects/WebCheckers/etc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCEA512-7FA0-5243-BFD0-BF21FFC893EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE9CA4F-0E1F-404E-8A39-2ADFD535E72C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16380" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="64">
   <si>
     <t>Instructions</t>
   </si>
@@ -134,9 +134,6 @@
     <t>D.R 10/03/2020</t>
   </si>
   <si>
-    <t>B.A. K.Z. 10/03/2020</t>
-  </si>
-  <si>
     <t>As a player I want to be able to move a piece on the board</t>
   </si>
   <si>
@@ -189,6 +186,42 @@
   </si>
   <si>
     <t>B.A. 10/19/2020</t>
+  </si>
+  <si>
+    <t>As a player, I want to be able to give out a code to non-players so they can spectate.</t>
+  </si>
+  <si>
+    <t>Given that I want to view a game, when I add a code in, then I expect to be taken to that particular game, such that I can spectate.</t>
+  </si>
+  <si>
+    <t>As the spectator, I want to see the moves as they happen live, and be able to differentiate between the two players.</t>
+  </si>
+  <si>
+    <t>Given that I am a spectator, if I am spectating the match, I want to see the match live and be able to tell which player is which.</t>
+  </si>
+  <si>
+    <t>As a player, I want to request help from spectators so that I can win the game.</t>
+  </si>
+  <si>
+    <t>Given that I am a player and want help, if I click the request help button, the spectators should get permission to highlight ways to go.</t>
+  </si>
+  <si>
+    <t>As a spectator, I want to be able to join a side of the game so that I can offer advise on moves.</t>
+  </si>
+  <si>
+    <t>Given I am a spectator, when one of the players requests for help, then I can decide whether or not to join.</t>
+  </si>
+  <si>
+    <t>As a spectator, I want to select a tile where a move can occur so that _BENEFIT_.</t>
+  </si>
+  <si>
+    <t>As a spectator, when I am allowed to help, I want to do so by highlighting a piece and a possible move they could take.</t>
+  </si>
+  <si>
+    <t>K.X.Z. 10/19/2020</t>
+  </si>
+  <si>
+    <t>B.A. K.X.Z. 10/03/2020</t>
   </si>
 </sst>
 </file>
@@ -737,7 +770,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
       <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F24" sqref="F24"/>
+      <selection pane="topRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -948,7 +981,7 @@
         <v>29</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="E13" s="8"/>
       <c r="G13" s="8"/>
@@ -990,17 +1023,17 @@
         <v>29</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="E16" s="8"/>
       <c r="G16" s="8"/>
     </row>
     <row r="17" spans="1:8" s="17" customFormat="1" ht="35" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>35</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>36</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="15"/>
@@ -1008,118 +1041,161 @@
         <v>29</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G17" s="16"/>
       <c r="H17" s="15"/>
     </row>
     <row r="18" spans="1:8" ht="85" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C18" s="8"/>
       <c r="E18" s="8" t="s">
         <v>29</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G18" s="8"/>
     </row>
     <row r="19" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="C19" s="8"/>
       <c r="E19" s="8" t="s">
         <v>29</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G19" s="8"/>
     </row>
     <row r="20" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="C20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="E20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="G20" s="8"/>
     </row>
     <row r="21" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="C21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="E21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="G21" s="8"/>
     </row>
     <row r="22" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="C22" s="8"/>
       <c r="E22" s="8" t="s">
         <v>29</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="C23" s="8"/>
       <c r="E23" s="8" t="s">
         <v>29</v>
       </c>
       <c r="F23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:8" s="17" customFormat="1" ht="52" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="G23" s="8"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="G24" s="8"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="15"/>
+    </row>
+    <row r="25" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="C25" s="8"/>
       <c r="E25" s="8"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="C26" s="8"/>
       <c r="E26" s="8"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="C27" s="8"/>
       <c r="E27" s="8"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="C28" s="8"/>
       <c r="E28" s="8"/>
       <c r="G28" s="8"/>

</xml_diff>